<commit_message>
新增CTF_Kalman_MINT_exp_ASPSO.m 和 obj_func_exp.m 來跑sorpos_estimation的臨近點之ASPSO JASA資料夾改成ICASSP_v2
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a0926\Desktop\碩班檔案\碩二上\CTF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\碩二上\CTF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B9276F-8ADF-4B42-8BC8-B0DCDFD7873E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C378F3FE-6828-48A0-A66E-6B56DF420A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5175" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.0000"/>
+    <numFmt numFmtId="176" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -168,7 +168,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1920,8 +1920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E55" sqref="B50:E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
simulation ULA+distributed 可行 明天把TIKR MPDR 加到CTF_combined之後開始跑其他T60  剩下baseline moving_source PSO 實驗數據補齊
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\碩二上\CTF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B1BF81-2E86-490C-B816-CE1AC3C4B40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14345572-A8FA-464D-825C-4070134F43DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>RLS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1970,33 +1970,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:N54"/>
+  <dimension ref="A3:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="15.42578125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="15.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="1"/>
+    <col min="14" max="14" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="N3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2012,8 +2027,23 @@
       <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>4096</v>
       </c>
@@ -2029,8 +2059,23 @@
       <c r="F5" s="1">
         <v>-12.410299999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O5" s="1">
+        <v>4096</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>-13.097799999999999</v>
+      </c>
+      <c r="R5" s="1">
+        <v>-13.889099999999999</v>
+      </c>
+      <c r="S5" s="1">
+        <v>-12.5974</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <f>B5+2048</f>
         <v>6144</v>
@@ -2048,8 +2093,16 @@
       <c r="F6" s="1">
         <v>-11.6999</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O6" s="1">
+        <f>O5+2048</f>
+        <v>6144</v>
+      </c>
+      <c r="P6" s="1">
+        <f>P5+0.1</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <f t="shared" ref="B7:B19" si="0">B6+2048</f>
         <v>8192</v>
@@ -2067,8 +2120,16 @@
       <c r="F7" s="1">
         <v>-10.9057</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O7" s="1">
+        <f t="shared" ref="O7:O19" si="2">O6+2048</f>
+        <v>8192</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" ref="P7:P14" si="3">P6+0.1</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <f t="shared" si="0"/>
         <v>10240</v>
@@ -2086,8 +2147,16 @@
       <c r="F8" s="1">
         <v>-10.8461</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O8" s="1">
+        <f t="shared" si="2"/>
+        <v>10240</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <f t="shared" si="0"/>
         <v>12288</v>
@@ -2105,8 +2174,16 @@
       <c r="F9" s="1">
         <v>-10.330299999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O9" s="1">
+        <f t="shared" si="2"/>
+        <v>12288</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>14336</v>
@@ -2124,8 +2201,16 @@
       <c r="F10" s="1">
         <v>-10.4254</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O10" s="1">
+        <f t="shared" si="2"/>
+        <v>14336</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>16384</v>
@@ -2143,8 +2228,16 @@
       <c r="F11" s="1">
         <v>-10.119</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O11" s="1">
+        <f t="shared" si="2"/>
+        <v>16384</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="3"/>
+        <v>0.79999999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>18432</v>
@@ -2162,8 +2255,16 @@
       <c r="F12" s="1">
         <v>-10.4375</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O12" s="1">
+        <f t="shared" si="2"/>
+        <v>18432</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="3"/>
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>20480</v>
@@ -2181,8 +2282,16 @@
       <c r="F13" s="1">
         <v>-11.363799999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O13" s="1">
+        <f t="shared" si="2"/>
+        <v>20480</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="3"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>22528</v>
@@ -2200,8 +2309,16 @@
       <c r="F14" s="1">
         <v>-11.5832</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O14" s="1">
+        <f t="shared" si="2"/>
+        <v>22528</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="3"/>
+        <v>1.0999999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>24576</v>
@@ -2219,14 +2336,22 @@
       <c r="F15" s="1">
         <v>-11.3993</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O15" s="1">
+        <f t="shared" si="2"/>
+        <v>24576</v>
+      </c>
+      <c r="P15" s="1">
+        <f>P14+0.1</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>26624</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" ref="C16" si="2">C15+0.1</f>
+        <f t="shared" ref="C16" si="4">C15+0.1</f>
         <v>1.3</v>
       </c>
       <c r="D16" s="1">
@@ -2238,8 +2363,16 @@
       <c r="F16" s="1">
         <v>-11.2187</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O16" s="1">
+        <f t="shared" si="2"/>
+        <v>26624</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" ref="P16" si="5">P15+0.1</f>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <f t="shared" si="0"/>
         <v>28672</v>
@@ -2257,8 +2390,16 @@
       <c r="F17" s="1">
         <v>-11.111599999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O17" s="1">
+        <f t="shared" si="2"/>
+        <v>28672</v>
+      </c>
+      <c r="P17" s="1">
+        <f>P16+0.1</f>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <f t="shared" si="0"/>
         <v>30720</v>
@@ -2276,14 +2417,22 @@
       <c r="F18" s="1">
         <v>-10.9763</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O18" s="1">
+        <f t="shared" si="2"/>
+        <v>30720</v>
+      </c>
+      <c r="P18" s="1">
+        <f>P17+0.1</f>
+        <v>1.5000000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <f t="shared" si="0"/>
         <v>32768</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" ref="C19" si="3">C18+0.1</f>
+        <f t="shared" ref="C19" si="6">C18+0.1</f>
         <v>1.6000000000000003</v>
       </c>
       <c r="D19" s="1">
@@ -2295,8 +2444,16 @@
       <c r="F19" s="1">
         <v>-10.4472</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="O19" s="1">
+        <f t="shared" si="2"/>
+        <v>32768</v>
+      </c>
+      <c r="P19" s="1">
+        <f t="shared" ref="P19" si="7">P18+0.1</f>
+        <v>1.6000000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
@@ -2304,7 +2461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
剩下CTF_combined T60=0.8~1    PSO  moving_source   evaluation metrics
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a0926\Desktop\碩班檔案\碩二上\CTF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00328C2-4636-4457-AA63-B1F0CB14237E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5260FE-4C8D-434C-B745-425B0C659D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="35">
   <si>
     <t>RLS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -192,6 +192,10 @@
   </si>
   <si>
     <t>RIR look_mic = 9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>look_mic = 9</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -275,13 +279,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2030,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:V56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="N55" sqref="N55"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2343,9 +2347,9 @@
         <f t="shared" si="3"/>
         <v>0.79999999999999993</v>
       </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
@@ -2373,9 +2377,9 @@
         <f t="shared" si="3"/>
         <v>0.89999999999999991</v>
       </c>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
@@ -2403,9 +2407,9 @@
         <f t="shared" si="3"/>
         <v>0.99999999999999989</v>
       </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
@@ -2433,9 +2437,15 @@
         <f t="shared" si="3"/>
         <v>1.0999999999999999</v>
       </c>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
+      <c r="Q14" s="7">
+        <v>-13.6486</v>
+      </c>
+      <c r="R14" s="7">
+        <v>-13.454499999999999</v>
+      </c>
+      <c r="S14" s="7">
+        <v>-13.3825</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
@@ -2463,9 +2473,15 @@
         <f>P14+0.1</f>
         <v>1.2</v>
       </c>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
+      <c r="Q15" s="7">
+        <v>-13.4506</v>
+      </c>
+      <c r="R15" s="7">
+        <v>-13.6967</v>
+      </c>
+      <c r="S15" s="7">
+        <v>-13.073700000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
@@ -2493,9 +2509,15 @@
         <f t="shared" ref="P16" si="5">P15+0.1</f>
         <v>1.3</v>
       </c>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
+      <c r="Q16" s="7">
+        <v>-13.0662</v>
+      </c>
+      <c r="R16" s="7">
+        <v>-13.059900000000001</v>
+      </c>
+      <c r="S16" s="7">
+        <v>-12.7338</v>
+      </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
@@ -2614,9 +2636,6 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="N24" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="O24" s="1" t="s">
         <v>5</v>
       </c>
@@ -2637,6 +2656,9 @@
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N25" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="O25" s="1">
         <v>256</v>
       </c>
@@ -2644,17 +2666,22 @@
         <v>0.01</v>
       </c>
       <c r="Q25" s="1">
-        <v>-12.0535</v>
+        <v>-9.3472000000000008</v>
       </c>
       <c r="R25" s="1">
-        <v>-11.2136</v>
+        <v>-9.0146999999999995</v>
       </c>
       <c r="S25" s="1">
-        <v>-11.914</v>
-      </c>
-      <c r="T25" s="5"/>
+        <v>-9.3560999999999996</v>
+      </c>
+      <c r="T25" s="7">
+        <v>-7.4119000000000002</v>
+      </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N26" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="O26" s="1">
         <v>1024</v>
       </c>
@@ -2670,7 +2697,9 @@
       <c r="S26" s="1">
         <v>-7.1623000000000001</v>
       </c>
-      <c r="T26" s="6"/>
+      <c r="T26" s="8">
+        <v>-2.9763E-7</v>
+      </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N29" s="1" t="s">
@@ -2845,7 +2874,7 @@
       <c r="Q38" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="R38" s="7"/>
+      <c r="R38" s="6"/>
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
@@ -2867,7 +2896,7 @@
       <c r="Q39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="R39" s="7"/>
+      <c r="R39" s="6"/>
     </row>
     <row r="40" spans="1:22" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
@@ -3048,9 +3077,9 @@
       <c r="R46" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="S46" s="7"/>
-      <c r="T46" s="7"/>
-      <c r="U46" s="7"/>
+      <c r="S46" s="6"/>
+      <c r="T46" s="6"/>
+      <c r="U46" s="6"/>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
@@ -3281,7 +3310,7 @@
       <c r="R56" s="1">
         <v>0.128</v>
       </c>
-      <c r="S56" s="8">
+      <c r="S56" s="7">
         <v>-1.2999999999999999E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
剩 application PSO moving_source
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a0926\Desktop\碩班檔案\碩二上\CTF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5260FE-4C8D-434C-B745-425B0C659D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A381CAC-86A9-410B-9497-0C3918E69965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="35">
   <si>
     <t>RLS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1172,7 +1172,1112 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW" sz="2000">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>NRMSPM</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="en-US" sz="2000">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wiener filter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$P$5:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$Q$5:$Q$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-9.3472000000000008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.1718999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-14.2432</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-14.391299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-14.7163</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-14.3667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-14.340299999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-14.282400000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-14.1173</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-13.784599999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-13.820399999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-13.6486</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-13.4506</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-13.0662</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-12.6869</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-12.952</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-12.766999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BC4E-4D33-9CB5-406D1C4D41EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$R$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RLS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$P$5:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$R$5:$R$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-9.0146999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.1848000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-14.963699999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-14.8531</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-14.792999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-14.581899999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-14.7172</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-14.491400000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-14.495900000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-13.960900000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-13.9497</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-13.454499999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-13.6967</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-13.059900000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-12.736599999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-12.573700000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-12.2751</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BC4E-4D33-9CB5-406D1C4D41EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$S$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kalman stationary filter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$P$5:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$S$5:$S$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-9.3560999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.1623000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13.515700000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-13.843299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-14.305099999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-13.872199999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-13.8901</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-13.9392</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-13.7197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-13.471500000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-13.4665</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-13.3825</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-13.073700000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-12.7338</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-12.3377</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-12.8581</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-12.729699999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BC4E-4D33-9CB5-406D1C4D41EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$T$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MCLMS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$P$5:$P$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$T$5:$T$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>-7.4119000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.9763E-7</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-BC4E-4D33-9CB5-406D1C4D41EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="460962751"/>
+        <c:axId val="460956511"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="460962751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.6"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1600" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>T</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1600" baseline="-25000">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>60</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1600" baseline="-25000">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.51244810307802435"/>
+              <c:y val="0.825857999139891"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="460956511"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="460956511"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2"/>
+          <c:min val="-18"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1600">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>dB</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1600">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="460962751"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.60301694274155981"/>
+          <c:y val="0.22287322141742025"/>
+          <c:w val="0.35011721074408764"/>
+          <c:h val="0.32579588551601729"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1728,20 +2833,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1761,6 +3382,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="圖表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01411942-FD2D-42AF-981D-6BAA58C65AF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2034,8 +3693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:V56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2060,7 +3719,7 @@
     <col min="23" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2074,7 +3733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2090,6 +3749,9 @@
       <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="N4" s="1" t="s">
         <v>27</v>
       </c>
@@ -2108,8 +3770,11 @@
       <c r="S4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="T4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>4096</v>
       </c>
@@ -2125,23 +3790,29 @@
       <c r="F5" s="1">
         <v>-12.410299999999999</v>
       </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
       <c r="O5" s="1">
-        <v>4096</v>
+        <v>256</v>
       </c>
       <c r="P5" s="1">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="Q5" s="1">
-        <v>-14.2432</v>
+        <v>-9.3472000000000008</v>
       </c>
       <c r="R5" s="1">
-        <v>-14.963699999999999</v>
+        <v>-9.0146999999999995</v>
       </c>
       <c r="S5" s="1">
-        <v>-13.515700000000001</v>
+        <v>-9.3560999999999996</v>
+      </c>
+      <c r="T5" s="7">
+        <v>-7.4119000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <f>B5+2048</f>
         <v>6144</v>
@@ -2159,25 +3830,29 @@
       <c r="F6" s="1">
         <v>-11.6999</v>
       </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
       <c r="O6" s="1">
-        <f>O5+2048</f>
-        <v>6144</v>
+        <v>1024</v>
       </c>
       <c r="P6" s="1">
-        <f>P5+0.1</f>
-        <v>0.30000000000000004</v>
+        <v>0.1</v>
       </c>
       <c r="Q6" s="1">
-        <v>-14.391299999999999</v>
+        <v>-7.1718999999999999</v>
       </c>
       <c r="R6" s="1">
-        <v>-14.8531</v>
+        <v>-6.1848000000000001</v>
       </c>
       <c r="S6" s="1">
-        <v>-13.843299999999999</v>
+        <v>-7.1623000000000001</v>
+      </c>
+      <c r="T6" s="8">
+        <v>-2.9763E-7</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <f t="shared" ref="B7:B19" si="0">B6+2048</f>
         <v>8192</v>
@@ -2195,25 +3870,29 @@
       <c r="F7" s="1">
         <v>-10.9057</v>
       </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
       <c r="O7" s="1">
-        <f t="shared" ref="O7:O19" si="2">O6+2048</f>
-        <v>8192</v>
+        <v>4096</v>
       </c>
       <c r="P7" s="1">
-        <f t="shared" ref="P7:P14" si="3">P6+0.1</f>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="Q7" s="1">
-        <v>-14.7163</v>
+        <v>-14.2432</v>
       </c>
       <c r="R7" s="1">
-        <v>-14.792999999999999</v>
+        <v>-14.963699999999999</v>
       </c>
       <c r="S7" s="1">
-        <v>-14.305099999999999</v>
+        <v>-13.515700000000001</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <f t="shared" si="0"/>
         <v>10240</v>
@@ -2231,25 +3910,31 @@
       <c r="F8" s="1">
         <v>-10.8461</v>
       </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
       <c r="O8" s="1">
-        <f t="shared" si="2"/>
-        <v>10240</v>
+        <f>O7+2048</f>
+        <v>6144</v>
       </c>
       <c r="P8" s="1">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
+        <f>P7+0.1</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="Q8" s="1">
-        <v>-14.3667</v>
+        <v>-14.391299999999999</v>
       </c>
       <c r="R8" s="1">
-        <v>-14.581899999999999</v>
+        <v>-14.8531</v>
       </c>
       <c r="S8" s="1">
-        <v>-13.872199999999999</v>
+        <v>-13.843299999999999</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <f t="shared" si="0"/>
         <v>12288</v>
@@ -2267,25 +3952,31 @@
       <c r="F9" s="1">
         <v>-10.330299999999999</v>
       </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
       <c r="O9" s="1">
-        <f t="shared" si="2"/>
-        <v>12288</v>
+        <f t="shared" ref="O7:O21" si="2">O8+2048</f>
+        <v>8192</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" si="3"/>
-        <v>0.6</v>
+        <f t="shared" ref="P7:P16" si="3">P8+0.1</f>
+        <v>0.4</v>
       </c>
       <c r="Q9" s="1">
-        <v>-14.340299999999999</v>
+        <v>-14.7163</v>
       </c>
       <c r="R9" s="1">
-        <v>-14.7172</v>
+        <v>-14.792999999999999</v>
       </c>
       <c r="S9" s="1">
-        <v>-13.8901</v>
+        <v>-14.305099999999999</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <f t="shared" si="0"/>
         <v>14336</v>
@@ -2303,25 +3994,31 @@
       <c r="F10" s="1">
         <v>-10.4254</v>
       </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
       <c r="O10" s="1">
         <f t="shared" si="2"/>
-        <v>14336</v>
+        <v>10240</v>
       </c>
       <c r="P10" s="1">
         <f t="shared" si="3"/>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="Q10" s="1">
-        <v>-14.282400000000001</v>
+        <v>-14.3667</v>
       </c>
       <c r="R10" s="1">
-        <v>-14.491400000000001</v>
+        <v>-14.581899999999999</v>
       </c>
       <c r="S10" s="1">
-        <v>-13.9392</v>
+        <v>-13.872199999999999</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <f t="shared" si="0"/>
         <v>16384</v>
@@ -2339,19 +4036,31 @@
       <c r="F11" s="1">
         <v>-10.119</v>
       </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
       <c r="O11" s="1">
         <f t="shared" si="2"/>
-        <v>16384</v>
+        <v>12288</v>
       </c>
       <c r="P11" s="1">
         <f t="shared" si="3"/>
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
+        <v>0.6</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>-14.340299999999999</v>
+      </c>
+      <c r="R11" s="1">
+        <v>-14.7172</v>
+      </c>
+      <c r="S11" s="1">
+        <v>-13.8901</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <f t="shared" si="0"/>
         <v>18432</v>
@@ -2369,19 +4078,31 @@
       <c r="F12" s="1">
         <v>-10.4375</v>
       </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
       <c r="O12" s="1">
         <f t="shared" si="2"/>
-        <v>18432</v>
+        <v>14336</v>
       </c>
       <c r="P12" s="1">
         <f t="shared" si="3"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
+        <v>0.7</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>-14.282400000000001</v>
+      </c>
+      <c r="R12" s="1">
+        <v>-14.491400000000001</v>
+      </c>
+      <c r="S12" s="1">
+        <v>-13.9392</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f t="shared" si="0"/>
         <v>20480</v>
@@ -2399,19 +4120,31 @@
       <c r="F13" s="1">
         <v>-11.363799999999999</v>
       </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
       <c r="O13" s="1">
         <f t="shared" si="2"/>
-        <v>20480</v>
+        <v>16384</v>
       </c>
       <c r="P13" s="1">
         <f t="shared" si="3"/>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="Q13" s="7">
+        <v>-14.1173</v>
+      </c>
+      <c r="R13" s="7">
+        <v>-14.495900000000001</v>
+      </c>
+      <c r="S13" s="7">
+        <v>-13.7197</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <f t="shared" si="0"/>
         <v>22528</v>
@@ -2429,25 +4162,31 @@
       <c r="F14" s="1">
         <v>-11.5832</v>
       </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
       <c r="O14" s="1">
         <f t="shared" si="2"/>
-        <v>22528</v>
+        <v>18432</v>
       </c>
       <c r="P14" s="1">
         <f t="shared" si="3"/>
-        <v>1.0999999999999999</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="Q14" s="7">
-        <v>-13.6486</v>
+        <v>-13.784599999999999</v>
       </c>
       <c r="R14" s="7">
-        <v>-13.454499999999999</v>
+        <v>-13.960900000000001</v>
       </c>
       <c r="S14" s="7">
-        <v>-13.3825</v>
+        <v>-13.471500000000001</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <f t="shared" si="0"/>
         <v>24576</v>
@@ -2465,25 +4204,31 @@
       <c r="F15" s="1">
         <v>-11.3993</v>
       </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
       <c r="O15" s="1">
         <f t="shared" si="2"/>
-        <v>24576</v>
+        <v>20480</v>
       </c>
       <c r="P15" s="1">
-        <f>P14+0.1</f>
-        <v>1.2</v>
+        <f t="shared" si="3"/>
+        <v>0.99999999999999989</v>
       </c>
       <c r="Q15" s="7">
-        <v>-13.4506</v>
+        <v>-13.820399999999999</v>
       </c>
       <c r="R15" s="7">
-        <v>-13.6967</v>
+        <v>-13.9497</v>
       </c>
       <c r="S15" s="7">
-        <v>-13.073700000000001</v>
+        <v>-13.4665</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <f t="shared" si="0"/>
         <v>26624</v>
@@ -2501,22 +4246,28 @@
       <c r="F16" s="1">
         <v>-11.2187</v>
       </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
       <c r="O16" s="1">
         <f t="shared" si="2"/>
-        <v>26624</v>
+        <v>22528</v>
       </c>
       <c r="P16" s="1">
-        <f t="shared" ref="P16" si="5">P15+0.1</f>
-        <v>1.3</v>
+        <f t="shared" si="3"/>
+        <v>1.0999999999999999</v>
       </c>
       <c r="Q16" s="7">
-        <v>-13.0662</v>
+        <v>-13.6486</v>
       </c>
       <c r="R16" s="7">
-        <v>-13.059900000000001</v>
+        <v>-13.454499999999999</v>
       </c>
       <c r="S16" s="7">
-        <v>-12.7338</v>
+        <v>-13.3825</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -2537,22 +4288,28 @@
       <c r="F17" s="1">
         <v>-11.111599999999999</v>
       </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
       <c r="O17" s="1">
         <f t="shared" si="2"/>
-        <v>28672</v>
+        <v>24576</v>
       </c>
       <c r="P17" s="1">
         <f>P16+0.1</f>
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>-12.6869</v>
-      </c>
-      <c r="R17" s="1">
-        <v>-12.736599999999999</v>
-      </c>
-      <c r="S17" s="1">
-        <v>-12.3377</v>
+        <v>1.2</v>
+      </c>
+      <c r="Q17" s="7">
+        <v>-13.4506</v>
+      </c>
+      <c r="R17" s="7">
+        <v>-13.6967</v>
+      </c>
+      <c r="S17" s="7">
+        <v>-13.073700000000001</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -2573,22 +4330,28 @@
       <c r="F18" s="1">
         <v>-10.9763</v>
       </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
       <c r="O18" s="1">
         <f t="shared" si="2"/>
-        <v>30720</v>
+        <v>26624</v>
       </c>
       <c r="P18" s="1">
-        <f>P17+0.1</f>
-        <v>1.5000000000000002</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>-12.952</v>
-      </c>
-      <c r="R18" s="1">
-        <v>-12.573700000000001</v>
-      </c>
-      <c r="S18" s="1">
-        <v>-12.8581</v>
+        <f t="shared" ref="P16:P18" si="5">P17+0.1</f>
+        <v>1.3</v>
+      </c>
+      <c r="Q18" s="7">
+        <v>-13.0662</v>
+      </c>
+      <c r="R18" s="7">
+        <v>-13.059900000000001</v>
+      </c>
+      <c r="S18" s="7">
+        <v>-12.7338</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -2609,22 +4372,72 @@
       <c r="F19" s="1">
         <v>-10.4472</v>
       </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
       <c r="O19" s="1">
         <f t="shared" si="2"/>
+        <v>28672</v>
+      </c>
+      <c r="P19" s="1">
+        <f>P18+0.1</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>-12.6869</v>
+      </c>
+      <c r="R19" s="1">
+        <v>-12.736599999999999</v>
+      </c>
+      <c r="S19" s="1">
+        <v>-12.3377</v>
+      </c>
+      <c r="T19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O20" s="1">
+        <f t="shared" si="2"/>
+        <v>30720</v>
+      </c>
+      <c r="P20" s="1">
+        <f>P19+0.1</f>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>-12.952</v>
+      </c>
+      <c r="R20" s="1">
+        <v>-12.573700000000001</v>
+      </c>
+      <c r="S20" s="1">
+        <v>-12.8581</v>
+      </c>
+      <c r="T20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O21" s="1">
+        <f t="shared" si="2"/>
         <v>32768</v>
       </c>
-      <c r="P19" s="1">
-        <f t="shared" ref="P19" si="7">P18+0.1</f>
+      <c r="P21" s="1">
+        <f t="shared" ref="P19:P21" si="7">P20+0.1</f>
         <v>1.6000000000000003</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="Q21" s="1">
         <v>-12.766999999999999</v>
       </c>
-      <c r="R19" s="1">
+      <c r="R21" s="1">
         <v>-12.2751</v>
       </c>
-      <c r="S19" s="1">
+      <c r="S21" s="1">
         <v>-12.729699999999999</v>
+      </c>
+      <c r="T21" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>